<commit_message>
Updated questions list, updated populate db for new models
</commit_message>
<xml_diff>
--- a/quizApp/data/DatasetsAndQuestions.xlsx
+++ b/quizApp/data/DatasetsAndQuestions.xlsx
@@ -168,7 +168,7 @@
     <t>answer_id</t>
   </si>
   <si>
-    <t>answer letter</t>
+    <t>answer_letter</t>
   </si>
   <si>
     <t>answer_text</t>
@@ -9745,7 +9745,7 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D1" s="1" t="s">

</xml_diff>